<commit_message>
changes w.r.t res and leaks
</commit_message>
<xml_diff>
--- a/irecodes-master/demand_damaged.xlsx
+++ b/irecodes-master/demand_damaged.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>N0</t>
   </si>
@@ -94,79 +94,160 @@
     <t>f0t7Leak</t>
   </si>
   <si>
+    <t>f1t0Leak</t>
+  </si>
+  <si>
     <t>f1t8Leak</t>
   </si>
   <si>
     <t>f1t2Leak</t>
   </si>
   <si>
+    <t>f2t1Leak</t>
+  </si>
+  <si>
     <t>f2t9Leak</t>
   </si>
   <si>
     <t>f2t3Leak</t>
   </si>
   <si>
+    <t>f3t2Leak</t>
+  </si>
+  <si>
     <t>f3t4Leak</t>
   </si>
   <si>
+    <t>f4t3Leak</t>
+  </si>
+  <si>
     <t>f4t11Leak</t>
   </si>
   <si>
     <t>f4t5Leak</t>
   </si>
   <si>
+    <t>f5t4Leak</t>
+  </si>
+  <si>
     <t>f5t6Leak</t>
   </si>
   <si>
     <t>f5t12Leak</t>
   </si>
   <si>
+    <t>f6t5Leak</t>
+  </si>
+  <si>
     <t>f6t13Leak</t>
   </si>
   <si>
+    <t>f7t0Leak</t>
+  </si>
+  <si>
     <t>f7t8Leak</t>
   </si>
   <si>
     <t>f7t14Leak</t>
   </si>
   <si>
+    <t>f8t7Leak</t>
+  </si>
+  <si>
+    <t>f8t1Leak</t>
+  </si>
+  <si>
     <t>f8t9Leak</t>
   </si>
   <si>
+    <t>f9t2Leak</t>
+  </si>
+  <si>
+    <t>f9t8Leak</t>
+  </si>
+  <si>
     <t>f9t16Leak</t>
   </si>
   <si>
+    <t>f11t4Leak</t>
+  </si>
+  <si>
     <t>f11t18Leak</t>
   </si>
   <si>
     <t>f11t12Leak</t>
   </si>
   <si>
+    <t>f12t5Leak</t>
+  </si>
+  <si>
+    <t>f12t11Leak</t>
+  </si>
+  <si>
     <t>f12t13Leak</t>
   </si>
   <si>
     <t>f12t19Leak</t>
   </si>
   <si>
+    <t>f13t6Leak</t>
+  </si>
+  <si>
+    <t>f13t12Leak</t>
+  </si>
+  <si>
     <t>f13t20Leak</t>
   </si>
   <si>
+    <t>f14t7Leak</t>
+  </si>
+  <si>
     <t>f14t15Leak</t>
   </si>
   <si>
+    <t>f15t14Leak</t>
+  </si>
+  <si>
     <t>f15t16Leak</t>
   </si>
   <si>
+    <t>f16t9Leak</t>
+  </si>
+  <si>
+    <t>f16t15Leak</t>
+  </si>
+  <si>
     <t>f16t17Leak</t>
   </si>
   <si>
+    <t>f17t16Leak</t>
+  </si>
+  <si>
     <t>f17t18Leak</t>
   </si>
   <si>
+    <t>f18t17Leak</t>
+  </si>
+  <si>
+    <t>f18t11Leak</t>
+  </si>
+  <si>
     <t>f18t19Leak</t>
   </si>
   <si>
+    <t>f19t18Leak</t>
+  </si>
+  <si>
+    <t>f19t12Leak</t>
+  </si>
+  <si>
     <t>f19t20Leak</t>
+  </si>
+  <si>
+    <t>f20t13Leak</t>
+  </si>
+  <si>
+    <t>f20t19Leak</t>
   </si>
   <si>
     <t>RES2</t>
@@ -536,13 +617,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD2"/>
+  <dimension ref="A1:CE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:56">
+    <row r="1" spans="1:83">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,8 +789,89 @@
       <c r="BD1" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="BE1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="2" spans="1:56">
+    <row r="2" spans="1:83">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -720,19 +882,19 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>7.431828617900139E-07</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>-0.002314814814815656</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.039832113255662E-06</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>-0.002314814814815656</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -765,10 +927,10 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>1.114773389494605E-06</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>-0.002314814814815656</v>
+        <v>0</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -780,10 +942,10 @@
         <v>0</v>
       </c>
       <c r="X2">
-        <v>3.466112704827206E-07</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>-0.002314814814815656</v>
+        <v>0</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -867,16 +1029,97 @@
         <v>0</v>
       </c>
       <c r="BA2">
-        <v>-0.03095693037639649</v>
+        <v>0</v>
       </c>
       <c r="BB2">
-        <v>-0.03095693035257963</v>
+        <v>0</v>
       </c>
       <c r="BC2">
-        <v>-0.03095693040823754</v>
+        <v>0</v>
       </c>
       <c r="BD2">
-        <v>-0.03095693028839684</v>
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
+        <v>0</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>0</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>0</v>
+      </c>
+      <c r="CA2">
+        <v>0</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+      <c r="CE2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>